<commit_message>
Top 5 Chart for Dashboard
</commit_message>
<xml_diff>
--- a/Xlookup_Examples.xlsx
+++ b/Xlookup_Examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Chandoo.org\Formulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\first\Data_Analysis_Using_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{6AC36118-2626-4A0C-ACEA-8378723B56BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AD073F6-1947-4B40-AEEE-5F3702BD1E8E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C232EE9C-994A-45F1-B87C-5C1D5C173544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C45B791-240C-4BDD-8DF1-1217944AF495}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{1C45B791-240C-4BDD-8DF1-1217944AF495}"/>
   </bookViews>
   <sheets>
     <sheet name="XLOOKUP" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,14 +37,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -157,7 +157,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,10 +651,10 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -665,13 +665,13 @@
     <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="49.5" customHeight="1">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
@@ -691,7 +691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
@@ -708,7 +708,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
@@ -732,7 +732,7 @@
         <v>43238</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
@@ -750,7 +750,7 @@
       </c>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
@@ -768,7 +768,7 @@
       </c>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
         <v>17</v>
       </c>
@@ -792,7 +792,7 @@
         <v>Dotty Strutley</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>19</v>
       </c>
@@ -810,7 +810,7 @@
       </c>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
@@ -828,7 +828,7 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
@@ -852,7 +852,7 @@
         <v>Ches Bonnell</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
         <v>21</v>
       </c>
@@ -869,7 +869,7 @@
         <v>58100</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
@@ -886,7 +886,7 @@
         <v>67910</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="9" t="s">
         <v>23</v>
       </c>
@@ -910,7 +910,7 @@
         <v>no such person</v>
       </c>
     </row>
-    <row r="17" spans="3:14">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="19" t="s">
         <v>24</v>
       </c>
@@ -927,7 +927,7 @@
         <v>41980</v>
       </c>
     </row>
-    <row r="18" spans="3:14">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
         <v>25</v>
       </c>
@@ -944,7 +944,7 @@
         <v>65920</v>
       </c>
     </row>
-    <row r="19" spans="3:14">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
         <v>26</v>
       </c>
@@ -977,7 +977,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="20" spans="3:14">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="9" t="s">
         <v>27</v>
       </c>
@@ -994,7 +994,7 @@
         <v>75970</v>
       </c>
     </row>
-    <row r="21" spans="3:14">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="9" t="s">
         <v>28</v>
       </c>
@@ -1024,7 +1024,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -1037,7 +1037,7 @@
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>43238</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>48950</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>74550</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>Jan Morforth</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>107700</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>88050</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>Kaine Padly</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>58100</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>67910</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>No such person</v>
       </c>
     </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
         <v>24</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>41980</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>65920</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>26</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>43355</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>75970</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>28</v>
       </c>

</xml_diff>